<commit_message>
Corrigido um erro no silkscren. Opino do MEM_R está invertido com o MEM_W
</commit_message>
<xml_diff>
--- a/Pinos Placa.xlsx
+++ b/Pinos Placa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\admg5\Documents\git\FPGAButtonBoard\FPGAButtonBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719F3916-4095-492C-8457-010687CE2296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE58B7CF-65A3-4D62-B246-C12515A70BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24660" yWindow="5700" windowWidth="7230" windowHeight="7755" xr2:uid="{FB73080F-9067-474D-9DEA-90F288873F74}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FB73080F-9067-474D-9DEA-90F288873F74}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -467,9 +467,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -478,6 +475,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,7 +795,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -818,553 +818,553 @@
       <c r="C1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>1</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>2</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4">
+        <v>4</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5">
-        <v>3</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="I3" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>5</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>6</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>7</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>8</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>9</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>10</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>11</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>12</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>13</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>14</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6" t="s">
+      <c r="H8" s="5"/>
+      <c r="I8" s="5" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>15</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>16</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6" t="s">
+      <c r="H9" s="5"/>
+      <c r="I9" s="5" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>17</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>18</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6" t="s">
+      <c r="H10" s="5"/>
+      <c r="I10" s="5" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>19</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>20</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6" t="s">
+      <c r="H11" s="5"/>
+      <c r="I11" s="5" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>21</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>22</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6" t="s">
+      <c r="H12" s="5"/>
+      <c r="I12" s="5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>23</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>24</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6" t="s">
+      <c r="H13" s="5"/>
+      <c r="I13" s="5" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>25</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>26</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6" t="s">
+      <c r="H14" s="5"/>
+      <c r="I14" s="5" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>27</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>28</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6" t="s">
+      <c r="H15" s="5"/>
+      <c r="I15" s="5" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>29</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <v>30</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>31</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>32</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6" t="s">
+      <c r="H17" s="5"/>
+      <c r="I17" s="5" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>33</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <v>34</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6" t="s">
+      <c r="H18" s="5"/>
+      <c r="I18" s="5" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>35</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>36</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6" t="s">
+      <c r="H19" s="5"/>
+      <c r="I19" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <v>37</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <v>38</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="G20" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6" t="s">
+      <c r="H20" s="5"/>
+      <c r="I20" s="5" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="4">
         <v>39</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="4">
         <v>40</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F21" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6" t="s">
+      <c r="H21" s="5"/>
+      <c r="I21" s="5" t="s">
         <v>109</v>
       </c>
     </row>

</xml_diff>